<commit_message>
Finished analysis for Prospectus
</commit_message>
<xml_diff>
--- a/raw-data/OtherData.xlsx
+++ b/raw-data/OtherData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gabe/Desktop/Projects/Gov94Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gabe/Desktop/Projects/Gov94Analysis/raw-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872A31C8-E055-084A-B26A-892898ABA76B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8C8B5D-30C5-6644-8392-D23FBCDB937C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2400" yWindow="3020" windowWidth="25640" windowHeight="14040" xr2:uid="{33E7C126-37A0-6D4E-9BBF-0058AD324F0A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="535">
   <si>
     <t>Aruba</t>
   </si>
@@ -1635,6 +1635,9 @@
   </si>
   <si>
     <t>code</t>
+  </si>
+  <si>
+    <t>GINI index (World Bank estimate) 2017</t>
   </si>
 </sst>
 </file>
@@ -1994,10 +1997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D6A769-183A-1348-AF8E-A43228ED1088}">
-  <dimension ref="A1:F265"/>
+  <dimension ref="A1:G265"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2006,7 +2009,7 @@
     <col min="5" max="5" width="56.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>532</v>
       </c>
@@ -2025,8 +2028,11 @@
       <c r="F1" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2035,7 +2041,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2055,7 +2061,7 @@
         <v>44.311116599999998</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2075,7 +2081,7 @@
         <v>49.724397000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2094,8 +2100,11 @@
       <c r="F5" s="1">
         <v>157.44310400000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>33.200000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2115,7 +2124,7 @@
         <v>1950.73515</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2135,7 +2144,7 @@
         <v>138.70242300000001</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -2155,7 +2164,7 @@
         <v>364.15482800000001</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2174,8 +2183,11 @@
       <c r="F9" s="1">
         <v>238.87967900000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <v>41.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2194,8 +2206,11 @@
       <c r="F10" s="1">
         <v>293.70543600000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10">
+        <v>33.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2207,7 +2222,7 @@
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -2227,7 +2242,7 @@
         <v>245.69887</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2247,7 +2262,7 @@
         <v>1585.3759399999999</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2266,8 +2281,11 @@
       <c r="F14" s="1">
         <v>1288.79106</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <v>29.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -2287,7 +2305,7 @@
         <v>213.61390900000001</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -2307,7 +2325,7 @@
         <v>5.9553655599999997</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -2326,8 +2344,11 @@
       <c r="F17" s="1">
         <v>659.51388499999996</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <v>27.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -2347,7 +2368,7 @@
         <v>14.895094800000001</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -2367,7 +2388,7 @@
         <v>14.923717999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -2387,7 +2408,7 @@
         <v>25.464336299999999</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -2406,8 +2427,11 @@
       <c r="F21" s="1">
         <v>302.78992399999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21">
+        <v>40.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -2427,7 +2451,7 @@
         <v>424.74746299999998</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -2447,7 +2471,7 @@
         <v>912.50204499999995</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -2467,7 +2491,7 @@
         <v>128.613663</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -2486,8 +2510,11 @@
       <c r="F25" s="1">
         <v>121.909734</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25">
+        <v>25.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -2507,7 +2534,7 @@
         <v>90.737018699999993</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>50</v>
       </c>
@@ -2516,7 +2543,7 @@
       </c>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -2535,8 +2562,11 @@
       <c r="F28" s="1">
         <v>66.169195200000004</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -2555,8 +2585,11 @@
       <c r="F29" s="1">
         <v>677.53614100000004</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29">
+        <v>53.3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -2576,7 +2609,7 @@
         <v>610.33539199999996</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -2596,7 +2629,7 @@
         <v>31.9829525</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>60</v>
       </c>
@@ -2615,8 +2648,11 @@
       <c r="F32" s="1">
         <v>19.441526</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32">
+        <v>37.4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>62</v>
       </c>
@@ -2636,7 +2672,7 @@
         <v>142.02640500000001</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>64</v>
       </c>
@@ -2656,7 +2692,7 @@
         <v>7.2303355600000003</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>66</v>
       </c>
@@ -2676,7 +2712,7 @@
         <v>1183.92615</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -2696,7 +2732,7 @@
         <v>236.84718699999999</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>70</v>
       </c>
@@ -2715,8 +2751,11 @@
       <c r="F37" s="1">
         <v>3660.9591099999998</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37">
+        <v>32.700000000000003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>72</v>
       </c>
@@ -2725,7 +2764,7 @@
       </c>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>74</v>
       </c>
@@ -2744,8 +2783,11 @@
       <c r="F39" s="1">
         <v>494.410504</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G39">
+        <v>44.4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>76</v>
       </c>
@@ -2765,7 +2807,7 @@
         <v>167.23201900000001</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>78</v>
       </c>
@@ -2785,7 +2827,7 @@
         <v>40.017626499999999</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>80</v>
       </c>
@@ -2805,7 +2847,7 @@
         <v>49.854146</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>82</v>
       </c>
@@ -2825,7 +2867,7 @@
         <v>9.1001583400000001</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -2845,7 +2887,7 @@
         <v>38.3122246</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>86</v>
       </c>
@@ -2864,8 +2906,11 @@
       <c r="F45" s="1">
         <v>123.745075</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G45">
+        <v>49.7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>88</v>
       </c>
@@ -2885,7 +2930,7 @@
         <v>44.062913700000003</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>90</v>
       </c>
@@ -2905,7 +2950,7 @@
         <v>44.783031800000003</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>92</v>
       </c>
@@ -2924,8 +2969,11 @@
       <c r="F48" s="1">
         <v>221.44331500000001</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G48">
+        <v>48.3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>94</v>
       </c>
@@ -2945,7 +2993,7 @@
         <v>251.814663</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>96</v>
       </c>
@@ -2965,7 +3013,7 @@
         <v>100.05244</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>98</v>
       </c>
@@ -2974,7 +3022,7 @@
       </c>
       <c r="F51" s="1"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>100</v>
       </c>
@@ -2983,7 +3031,7 @@
       </c>
       <c r="F52" s="1"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>102</v>
       </c>
@@ -3002,8 +3050,11 @@
       <c r="F53" s="1">
         <v>925.63458700000001</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G53">
+        <v>31.4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>104</v>
       </c>
@@ -3022,8 +3073,11 @@
       <c r="F54" s="1">
         <v>239.499809</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G54">
+        <v>24.9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>106</v>
       </c>
@@ -3043,7 +3097,7 @@
         <v>722.65743399999997</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>108</v>
       </c>
@@ -3059,8 +3113,11 @@
       <c r="F56" s="1">
         <v>18.531087400000001</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G56">
+        <v>41.6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>110</v>
       </c>
@@ -3080,7 +3137,7 @@
         <v>127.271745</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>112</v>
       </c>
@@ -3099,8 +3156,11 @@
       <c r="F58" s="1">
         <v>883.68177200000002</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G58">
+        <v>28.7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>114</v>
       </c>
@@ -3119,8 +3179,11 @@
       <c r="F59" s="1">
         <v>222.236817</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G59">
+        <v>42.2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>116</v>
       </c>
@@ -3140,7 +3203,7 @@
         <v>84.086032299999999</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>118</v>
       </c>
@@ -3160,7 +3223,7 @@
         <v>134.86618200000001</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>120</v>
       </c>
@@ -3180,7 +3243,7 @@
         <v>75.183107100000001</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>122</v>
       </c>
@@ -3200,7 +3263,7 @@
         <v>202.10351199999999</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>124</v>
       </c>
@@ -3220,7 +3283,7 @@
         <v>144.46257399999999</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>126</v>
       </c>
@@ -3240,7 +3303,7 @@
         <v>467.07045099999999</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>128</v>
       </c>
@@ -3259,8 +3322,11 @@
       <c r="F66" s="1">
         <v>244.525814</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G66">
+        <v>44.7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>130</v>
       </c>
@@ -3279,8 +3345,11 @@
       <c r="F67" s="1">
         <v>91.267337800000007</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G67">
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>132</v>
       </c>
@@ -3300,7 +3369,7 @@
         <v>726.09876999999994</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>134</v>
       </c>
@@ -3317,7 +3386,7 @@
         <v>17.653454199999999</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>136</v>
       </c>
@@ -3336,8 +3405,11 @@
       <c r="F70" s="1">
         <v>687.38007200000004</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G70">
+        <v>34.700000000000003</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>138</v>
       </c>
@@ -3356,8 +3428,11 @@
       <c r="F71" s="1">
         <v>288.764995</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G71">
+        <v>30.4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>140</v>
       </c>
@@ -3377,7 +3452,7 @@
         <v>15.7061999</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>142</v>
       </c>
@@ -3397,7 +3472,7 @@
         <v>651.37402599999996</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>144</v>
       </c>
@@ -3417,7 +3492,7 @@
         <v>45.855473699999997</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>146</v>
       </c>
@@ -3436,8 +3511,11 @@
       <c r="F75" s="1">
         <v>932.08530199999996</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G75">
+        <v>27.4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>148</v>
       </c>
@@ -3457,7 +3535,7 @@
         <v>59.387873300000003</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>150</v>
       </c>
@@ -3476,8 +3554,11 @@
       <c r="F77" s="1">
         <v>729.20424100000002</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G77">
+        <v>31.6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>152</v>
       </c>
@@ -3486,7 +3567,7 @@
       </c>
       <c r="F78" s="1"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>154</v>
       </c>
@@ -3506,7 +3587,7 @@
         <v>11.2866286</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>156</v>
       </c>
@@ -3525,8 +3606,11 @@
       <c r="F80" s="1">
         <v>76.151050900000001</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G80">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>158</v>
       </c>
@@ -3546,7 +3630,7 @@
         <v>782.28635499999996</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>160</v>
       </c>
@@ -3565,8 +3649,11 @@
       <c r="F82" s="1">
         <v>188.477045</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G82">
+        <v>37.9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>162</v>
       </c>
@@ -3586,7 +3673,7 @@
         <v>32.980383400000001</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>164</v>
       </c>
@@ -3595,7 +3682,7 @@
       </c>
       <c r="F84" s="1"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>166</v>
       </c>
@@ -3615,7 +3702,7 @@
         <v>22.651069499999998</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>168</v>
       </c>
@@ -3635,7 +3722,7 @@
         <v>7.8690768000000002</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>170</v>
       </c>
@@ -3655,7 +3742,7 @@
         <v>13.825374</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>172</v>
       </c>
@@ -3675,7 +3762,7 @@
         <v>211.76019400000001</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>174</v>
       </c>
@@ -3694,8 +3781,11 @@
       <c r="F89" s="1">
         <v>589.18918799999994</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G89">
+        <v>34.4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>176</v>
       </c>
@@ -3715,7 +3805,7 @@
         <v>298.36815999999999</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>178</v>
       </c>
@@ -3727,7 +3817,7 @@
       </c>
       <c r="F91" s="1"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>180</v>
       </c>
@@ -3747,7 +3837,7 @@
         <v>149.28843599999999</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>182</v>
       </c>
@@ -3759,7 +3849,7 @@
       </c>
       <c r="F93" s="1"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>184</v>
       </c>
@@ -3779,7 +3869,7 @@
         <v>67.5923224</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>186</v>
       </c>
@@ -3799,7 +3889,7 @@
         <v>1038.5689</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>188</v>
       </c>
@@ -3811,7 +3901,7 @@
       </c>
       <c r="F96" s="1"/>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>190</v>
       </c>
@@ -3830,8 +3920,11 @@
       <c r="F97" s="1">
         <v>101.65693899999999</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G97">
+        <v>50.5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>192</v>
       </c>
@@ -3851,7 +3944,7 @@
         <v>26.030795699999999</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>194</v>
       </c>
@@ -3870,8 +3963,11 @@
       <c r="F99" s="1">
         <v>192.40727699999999</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G99">
+        <v>30.4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>196</v>
       </c>
@@ -3891,7 +3987,7 @@
         <v>17.458354499999999</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>198</v>
       </c>
@@ -3910,8 +4006,11 @@
       <c r="F101" s="1">
         <v>321.76916599999998</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G101">
+        <v>30.6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>200</v>
       </c>
@@ -3931,7 +4030,7 @@
         <v>142.60432599999999</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>202</v>
       </c>
@@ -3951,7 +4050,7 @@
         <v>115.804895</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>204</v>
       </c>
@@ -3971,7 +4070,7 @@
         <v>32.535769799999997</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>206</v>
       </c>
@@ -3991,7 +4090,7 @@
         <v>43.157630099999999</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>208</v>
       </c>
@@ -4010,8 +4109,11 @@
       <c r="F106" s="1">
         <v>61.1779394</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G106">
+        <v>39.4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>210</v>
       </c>
@@ -4031,7 +4133,7 @@
         <v>26.6902139</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>212</v>
       </c>
@@ -4040,7 +4142,7 @@
       </c>
       <c r="F108" s="1"/>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>214</v>
       </c>
@@ -4060,7 +4162,7 @@
         <v>46.126995200000003</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>216</v>
       </c>
@@ -4069,7 +4171,7 @@
       </c>
       <c r="F110" s="1"/>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>218</v>
       </c>
@@ -4089,7 +4191,7 @@
         <v>1329.079</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>220</v>
       </c>
@@ -4105,8 +4207,11 @@
       <c r="F112" s="1">
         <v>188.73728399999999</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G112">
+        <v>40.799999999999997</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>222</v>
       </c>
@@ -4126,7 +4231,7 @@
         <v>119.82399599999999</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>224</v>
       </c>
@@ -4146,7 +4251,7 @@
         <v>936.25634700000001</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>226</v>
       </c>
@@ -4166,7 +4271,7 @@
         <v>1020.5247900000001</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>228</v>
       </c>
@@ -4185,8 +4290,11 @@
       <c r="F116" s="1">
         <v>699.35002699999995</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G116">
+        <v>35.9</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>230</v>
       </c>
@@ -4206,7 +4314,7 @@
         <v>113.412892</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>232</v>
       </c>
@@ -4226,7 +4334,7 @@
         <v>69.4578633</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>234</v>
       </c>
@@ -4246,7 +4354,7 @@
         <v>694.82376899999997</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>236</v>
       </c>
@@ -4265,8 +4373,11 @@
       <c r="F120" s="1">
         <v>104.898669</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G120">
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>238</v>
       </c>
@@ -4286,7 +4397,7 @@
         <v>29.374262099999999</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>240</v>
       </c>
@@ -4305,8 +4416,11 @@
       <c r="F122" s="1">
         <v>41.975760800000003</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G122">
+        <v>27.3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>242</v>
       </c>
@@ -4326,7 +4440,7 @@
         <v>46.016420199999999</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>244</v>
       </c>
@@ -4346,7 +4460,7 @@
         <v>4.8443375900000003</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>246</v>
       </c>
@@ -4366,7 +4480,7 @@
         <v>528.95257500000002</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>248</v>
       </c>
@@ -4386,7 +4500,7 @@
         <v>834.81697899999995</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>250</v>
       </c>
@@ -4406,7 +4520,7 @@
         <v>172.12068400000001</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>252</v>
       </c>
@@ -4426,7 +4540,7 @@
         <v>356.55911800000001</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>254</v>
       </c>
@@ -4446,7 +4560,7 @@
         <v>27.319454499999999</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>256</v>
       </c>
@@ -4466,7 +4580,7 @@
         <v>311.381979</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>258</v>
       </c>
@@ -4486,7 +4600,7 @@
         <v>37.784549300000002</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>260</v>
       </c>
@@ -4498,7 +4612,7 @@
       </c>
       <c r="F132" s="1"/>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>262</v>
       </c>
@@ -4518,7 +4632,7 @@
         <v>265.73206099999999</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>264</v>
       </c>
@@ -4538,7 +4652,7 @@
         <v>361.73157400000002</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>266</v>
       </c>
@@ -4558,7 +4672,7 @@
         <v>25.459591799999998</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>268</v>
       </c>
@@ -4578,7 +4692,7 @@
         <v>15.8152553</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>270</v>
       </c>
@@ -4587,7 +4701,7 @@
       </c>
       <c r="F137" s="1"/>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>272</v>
       </c>
@@ -4607,7 +4721,7 @@
         <v>85.4473354</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>274</v>
       </c>
@@ -4627,7 +4741,7 @@
         <v>51.20102</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>276</v>
       </c>
@@ -4647,7 +4761,7 @@
         <v>113.392236</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>278</v>
       </c>
@@ -4666,8 +4780,11 @@
       <c r="F141" s="1">
         <v>16.150731199999999</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G141">
+        <v>44.9</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>280</v>
       </c>
@@ -4687,7 +4804,7 @@
         <v>213.49453800000001</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>282</v>
       </c>
@@ -4706,8 +4823,11 @@
       <c r="F143" s="1">
         <v>330.10642999999999</v>
       </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G143">
+        <v>37.299999999999997</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>284</v>
       </c>
@@ -4726,8 +4846,11 @@
       <c r="F144" s="1">
         <v>1105.51226</v>
       </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G144">
+        <v>34.9</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>286</v>
       </c>
@@ -4746,8 +4869,11 @@
       <c r="F145" s="1">
         <v>396.60366499999998</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G145">
+        <v>35.6</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>288</v>
       </c>
@@ -4759,7 +4885,7 @@
       </c>
       <c r="F146" s="1"/>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>290</v>
       </c>
@@ -4768,7 +4894,7 @@
       </c>
       <c r="F147" s="1"/>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>292</v>
       </c>
@@ -4788,7 +4914,7 @@
         <v>89.999079499999993</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>294</v>
       </c>
@@ -4808,7 +4934,7 @@
         <v>601.03353700000002</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>296</v>
       </c>
@@ -4827,8 +4953,11 @@
       <c r="F150" s="1">
         <v>81.314429000000004</v>
       </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G150">
+        <v>25.9</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>298</v>
       </c>
@@ -4848,7 +4977,7 @@
         <v>6.5805433899999999</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>300</v>
       </c>
@@ -4868,7 +4997,7 @@
         <v>282.77915899999999</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>302</v>
       </c>
@@ -4888,7 +5017,7 @@
         <v>173.543868</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>304</v>
       </c>
@@ -4908,7 +5037,7 @@
         <v>220.97434100000001</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>306</v>
       </c>
@@ -4928,7 +5057,7 @@
         <v>101.948517</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>308</v>
       </c>
@@ -4948,7 +5077,7 @@
         <v>123.568609</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>310</v>
       </c>
@@ -4967,8 +5096,11 @@
       <c r="F157" s="1">
         <v>117.06820500000001</v>
       </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G157">
+        <v>34.200000000000003</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>312</v>
       </c>
@@ -4988,7 +5120,7 @@
         <v>10.791159499999999</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>314</v>
       </c>
@@ -5007,8 +5139,11 @@
       <c r="F159" s="1">
         <v>858.69678299999998</v>
       </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G159">
+        <v>29.2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>316</v>
       </c>
@@ -5027,8 +5162,11 @@
       <c r="F160" s="1">
         <v>45.949944100000003</v>
       </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G160">
+        <v>30.7</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>318</v>
       </c>
@@ -5045,7 +5183,7 @@
         <v>122.684315</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>320</v>
       </c>
@@ -5065,7 +5203,7 @@
         <v>130.474841</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>322</v>
       </c>
@@ -5085,7 +5223,7 @@
         <v>55.464607100000002</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>324</v>
       </c>
@@ -5097,7 +5235,7 @@
       </c>
       <c r="F164" s="1"/>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>326</v>
       </c>
@@ -5117,7 +5255,7 @@
         <v>1.6415403200000001</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>328</v>
       </c>
@@ -5137,7 +5275,7 @@
         <v>25.788370199999999</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>330</v>
       </c>
@@ -5156,8 +5294,11 @@
       <c r="F167" s="1">
         <v>307.86186900000001</v>
       </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G167">
+        <v>36.799999999999997</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>332</v>
       </c>
@@ -5177,7 +5318,7 @@
         <v>5.3835251299999998</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>334</v>
       </c>
@@ -5197,7 +5338,7 @@
         <v>178.981539</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>336</v>
       </c>
@@ -5217,7 +5358,7 @@
         <v>1730.7035599999999</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>338</v>
       </c>
@@ -5237,7 +5378,7 @@
         <v>125.284588</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>340</v>
       </c>
@@ -5246,7 +5387,7 @@
       </c>
       <c r="F172" s="1"/>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>342</v>
       </c>
@@ -5266,7 +5407,7 @@
         <v>14.234654600000001</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>344</v>
       </c>
@@ -5286,7 +5427,7 @@
         <v>60.831387300000003</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>346</v>
       </c>
@@ -5306,7 +5447,7 @@
         <v>64.064565599999995</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>348</v>
       </c>
@@ -5325,8 +5466,11 @@
       <c r="F176" s="1">
         <v>902.09952499999997</v>
       </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G176">
+        <v>28.5</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>350</v>
       </c>
@@ -5345,8 +5489,11 @@
       <c r="F177" s="1">
         <v>1111.94739</v>
       </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G177">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>352</v>
       </c>
@@ -5366,7 +5513,7 @@
         <v>31.686446700000001</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>354</v>
       </c>
@@ -5386,7 +5533,7 @@
         <v>48.432460200000001</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>356</v>
       </c>
@@ -5406,7 +5553,7 @@
         <v>799.45596999999998</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>358</v>
       </c>
@@ -5426,7 +5573,7 @@
         <v>939.75117299999999</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>360</v>
       </c>
@@ -5446,7 +5593,7 @@
         <v>70.392616799999999</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>362</v>
       </c>
@@ -5466,7 +5613,7 @@
         <v>187.48467400000001</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>364</v>
       </c>
@@ -5486,7 +5633,7 @@
         <v>26.920686</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>366</v>
       </c>
@@ -5505,8 +5652,11 @@
       <c r="F185" s="1">
         <v>350.37804599999998</v>
       </c>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G185">
+        <v>49.9</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>368</v>
       </c>
@@ -5525,8 +5675,11 @@
       <c r="F186" s="1">
         <v>112.820082</v>
       </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G186">
+        <v>43.3</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>370</v>
       </c>
@@ -5546,7 +5699,7 @@
         <v>85.778288099999997</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>372</v>
       </c>
@@ -5566,7 +5719,7 @@
         <v>416.49296900000002</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>374</v>
       </c>
@@ -5586,7 +5739,7 @@
         <v>4.3310809600000004</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>376</v>
       </c>
@@ -5605,8 +5758,11 @@
       <c r="F190" s="1">
         <v>243.68364800000001</v>
       </c>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G190">
+        <v>29.7</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>378</v>
       </c>
@@ -5626,7 +5782,7 @@
         <v>38.726007500000001</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>380</v>
       </c>
@@ -5638,7 +5794,7 @@
       </c>
       <c r="F192" s="1"/>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>382</v>
       </c>
@@ -5647,7 +5803,7 @@
       </c>
       <c r="F193" s="1"/>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>384</v>
       </c>
@@ -5666,8 +5822,11 @@
       <c r="F194" s="1">
         <v>605.91570100000001</v>
       </c>
-    </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G194">
+        <v>33.799999999999997</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>386</v>
       </c>
@@ -5686,8 +5845,11 @@
       <c r="F195" s="1">
         <v>158.14306300000001</v>
       </c>
-    </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G195">
+        <v>48.8</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>388</v>
       </c>
@@ -5699,7 +5861,7 @@
       </c>
       <c r="F196" s="1"/>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>390</v>
       </c>
@@ -5719,7 +5881,7 @@
         <v>34.717853300000002</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>392</v>
       </c>
@@ -5739,7 +5901,7 @@
         <v>1056.5295599999999</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>394</v>
       </c>
@@ -5748,7 +5910,7 @@
       </c>
       <c r="F199" s="1"/>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>396</v>
       </c>
@@ -5768,7 +5930,7 @@
         <v>335.66936099999998</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>398</v>
       </c>
@@ -5787,8 +5949,11 @@
       <c r="F201" s="1">
         <v>103.90602199999999</v>
       </c>
-    </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G201">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>400</v>
       </c>
@@ -5807,8 +5972,11 @@
       <c r="F202" s="1">
         <v>201.96062000000001</v>
       </c>
-    </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G202">
+        <v>37.200000000000003</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>402</v>
       </c>
@@ -5828,7 +5996,7 @@
         <v>7.4634308899999997</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>404</v>
       </c>
@@ -5848,7 +6016,7 @@
         <v>42.340586799999997</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>406</v>
       </c>
@@ -5868,7 +6036,7 @@
         <v>369.42557900000003</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>408</v>
       </c>
@@ -5888,7 +6056,7 @@
         <v>119.03195599999999</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>410</v>
       </c>
@@ -5908,7 +6076,7 @@
         <v>31.1716029</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>412</v>
       </c>
@@ -5928,7 +6096,7 @@
         <v>1119.76937</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>414</v>
       </c>
@@ -5948,7 +6116,7 @@
         <v>4.8947647700000001</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>416</v>
       </c>
@@ -5968,7 +6136,7 @@
         <v>41.284288400000001</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>418</v>
       </c>
@@ -5987,8 +6155,11 @@
       <c r="F211" s="1">
         <v>97.786021599999998</v>
       </c>
-    </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G211">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>420</v>
       </c>
@@ -6005,7 +6176,7 @@
         <v>590.80740000000003</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>422</v>
       </c>
@@ -6014,7 +6185,7 @@
       </c>
       <c r="F213" s="1"/>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>424</v>
       </c>
@@ -6033,8 +6204,11 @@
       <c r="F214" s="1">
         <v>206.915414</v>
       </c>
-    </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G214">
+        <v>36.200000000000003</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>426</v>
       </c>
@@ -6054,7 +6228,7 @@
         <v>41.785460499999999</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>428</v>
       </c>
@@ -6063,7 +6237,7 @@
       </c>
       <c r="F216" s="1"/>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>430</v>
       </c>
@@ -6083,7 +6257,7 @@
         <v>41.782717099999999</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>432</v>
       </c>
@@ -6103,7 +6277,7 @@
         <v>190.10671400000001</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>434</v>
       </c>
@@ -6122,8 +6296,11 @@
       <c r="F219" s="1">
         <v>16.298585899999999</v>
       </c>
-    </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G219">
+        <v>56.3</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>436</v>
       </c>
@@ -6143,7 +6320,7 @@
         <v>104.144268</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>438</v>
       </c>
@@ -6163,7 +6340,7 @@
         <v>237.640604</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>440</v>
       </c>
@@ -6182,8 +6359,11 @@
       <c r="F222" s="1">
         <v>508.28729199999998</v>
       </c>
-    </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G222">
+        <v>24.2</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>442</v>
       </c>
@@ -6202,8 +6382,11 @@
       <c r="F223" s="1">
         <v>941.93647899999996</v>
       </c>
-    </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G223">
+        <v>28.8</v>
+      </c>
+    </row>
+    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>444</v>
       </c>
@@ -6223,7 +6406,7 @@
         <v>37.280501200000003</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>446</v>
       </c>
@@ -6232,7 +6415,7 @@
       </c>
       <c r="F225" s="1"/>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>448</v>
       </c>
@@ -6252,7 +6435,7 @@
         <v>12.881612199999999</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>450</v>
       </c>
@@ -6261,7 +6444,7 @@
       </c>
       <c r="F227" s="1"/>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>452</v>
       </c>
@@ -6270,7 +6453,7 @@
       </c>
       <c r="F228" s="1"/>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>454</v>
       </c>
@@ -6290,7 +6473,7 @@
         <v>21.086427100000002</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>456</v>
       </c>
@@ -6310,7 +6493,7 @@
         <v>134.86864399999999</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>458</v>
       </c>
@@ -6330,7 +6513,7 @@
         <v>153.20769899999999</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>460</v>
       </c>
@@ -6350,7 +6533,7 @@
         <v>22.963280999999998</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>462</v>
       </c>
@@ -6369,8 +6552,11 @@
       <c r="F233" s="1">
         <v>48.005816799999998</v>
       </c>
-    </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G233">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>464</v>
       </c>
@@ -6390,7 +6576,7 @@
         <v>36.921033000000001</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>466</v>
       </c>
@@ -6410,7 +6596,7 @@
         <v>343.659133</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>468</v>
       </c>
@@ -6430,7 +6616,7 @@
         <v>366.33716700000002</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>470</v>
       </c>
@@ -6450,7 +6636,7 @@
         <v>10.0577691</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>472</v>
       </c>
@@ -6467,7 +6653,7 @@
         <v>122.684315</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>474</v>
       </c>
@@ -6487,7 +6673,7 @@
         <v>29.914274200000001</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>476</v>
       </c>
@@ -6507,7 +6693,7 @@
         <v>42.340586799999997</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>478</v>
       </c>
@@ -6527,7 +6713,7 @@
         <v>41.782717099999999</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>480</v>
       </c>
@@ -6547,7 +6733,7 @@
         <v>501.39288800000003</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>482</v>
       </c>
@@ -6567,7 +6753,7 @@
         <v>111.06304299999999</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>484</v>
       </c>
@@ -6586,8 +6772,11 @@
       <c r="F244" s="1">
         <v>101.030131</v>
       </c>
-    </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G244">
+        <v>41.4</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>486</v>
       </c>
@@ -6607,7 +6796,7 @@
         <v>16.876530299999999</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>488</v>
       </c>
@@ -6626,8 +6815,11 @@
       <c r="F246" s="1">
         <v>8.1510944999999992</v>
       </c>
-    </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G246">
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>490</v>
       </c>
@@ -6647,7 +6839,7 @@
         <v>16.195336300000001</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>492</v>
       </c>
@@ -6666,8 +6858,11 @@
       <c r="F248" s="1">
         <v>80.138608099999999</v>
       </c>
-    </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G248">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="249" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>494</v>
       </c>
@@ -6687,7 +6882,7 @@
         <v>205.91970900000001</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>496</v>
       </c>
@@ -6706,8 +6901,11 @@
       <c r="F250" s="1">
         <v>389.84339299999999</v>
       </c>
-    </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G250">
+        <v>39.5</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>498</v>
       </c>
@@ -6727,7 +6925,7 @@
         <v>1791.81654</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>500</v>
       </c>
@@ -6747,7 +6945,7 @@
         <v>71.191800299999997</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>502</v>
       </c>
@@ -6767,7 +6965,7 @@
         <v>56.6247513</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>504</v>
       </c>
@@ -6785,7 +6983,7 @@
       </c>
       <c r="F254" s="1"/>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>506</v>
       </c>
@@ -6794,7 +6992,7 @@
       </c>
       <c r="F255" s="1"/>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>508</v>
       </c>
@@ -6803,7 +7001,7 @@
       </c>
       <c r="F256" s="1"/>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>510</v>
       </c>
@@ -6823,7 +7021,7 @@
         <v>59.578136299999997</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>512</v>
       </c>
@@ -6843,7 +7041,7 @@
         <v>12.645607</v>
       </c>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>514</v>
       </c>
@@ -6863,7 +7061,7 @@
         <v>261.59254199999998</v>
       </c>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>516</v>
       </c>
@@ -6883,7 +7081,7 @@
         <v>29.049634399999999</v>
       </c>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>518</v>
       </c>
@@ -6894,8 +7092,11 @@
         <v>7678890905.2334747</v>
       </c>
       <c r="F261" s="1"/>
-    </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G261">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="262" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>520</v>
       </c>
@@ -6907,7 +7108,7 @@
       </c>
       <c r="F262" s="1"/>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>522</v>
       </c>
@@ -6927,7 +7128,7 @@
         <v>189.55792099999999</v>
       </c>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>524</v>
       </c>
@@ -6947,7 +7148,7 @@
         <v>10.865031699999999</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>526</v>
       </c>
@@ -6965,6 +7166,9 @@
       </c>
       <c r="F265" s="1">
         <v>26.374036700000001</v>
+      </c>
+      <c r="G265">
+        <v>44.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>